<commit_message>
Added data transformation methods
</commit_message>
<xml_diff>
--- a/data/answer_sheet.xlsx
+++ b/data/answer_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UU\Year 2\Period 2\Advanced Research Methods (ARM)\Data Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F4EB5D2-4160-445F-9BD8-11FA8F74FC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE679F9-3580-4300-9F39-F98A3EF86AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Q1.1</t>
   </si>
@@ -97,16 +97,26 @@
   </si>
   <si>
     <t>Q3.5</t>
+  </si>
+  <si>
+    <t>Q2.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,126 +428,126 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="b">
+      <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B2" t="b">
+      <c r="B2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C2" t="b">
+      <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2">
+      <c r="K2" s="1">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="M2" s="1">
         <v>3</v>
       </c>
-      <c r="H2">
+      <c r="N2" s="1">
         <v>4</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="N2">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>